<commit_message>
[NOREA - DORA in Control Framework V3.0] Fix French Version
- Excel file only : Added a note indicating that the French version isn't official
</commit_message>
<xml_diff>
--- a/tools/excel/dora/norea.xlsx
+++ b/tools/excel/dora/norea.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\dora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AE967E-8445-4CB8-8862-34CD3B1E7430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C1A82C-7308-42D0-B7AC-8B97858415BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10410" yWindow="-21710" windowWidth="38620" windowHeight="21820" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -1314,10 +1314,6 @@
     <t>NOREA - DORA en Control Framework V3.0</t>
   </si>
   <si>
-    <t>NOREA - DORA en Control Framework est un outil pratique conçu pour aider les organisations à se conformer à la loi sur la résilience opérationnelle numérique (DORA). Bien que ce cadre offre des indications précieuses, il est important de noter que les exigences juridiques énoncées dans la DORA elle-même restent de premier plan.
-Lien : https://www.norea.nl/dora</t>
-  </si>
-  <si>
     <t>NOREA - DORA en Control Framework et le tableau de bord est sous licence Creative Commons BY 4.0. Pour plus d’informations :
 https://creativecommons.org/licenses/by/4.0/
 Vous êtes libre de :
@@ -2141,6 +2137,11 @@
 ▪ Les mesures de contrôle en place sont comparées à des données externes et constituent des « pratiques exemplaires » par rapport à celles d’autres organisations.
 ▪ L’évaluation de l’efficacité de l’application de la mesure de contrôle est fondée sur des CIP (métriques).
 ▪ Il est prouvé que les employés sont impliqués en permanence et de manière proactive dans l’amélioration des mesures de contrôle.</t>
+  </si>
+  <si>
+    <t>[Traduction non officielle]
+NOREA - DORA en Control Framework est un outil pratique conçu pour aider les organisations à se conformer à la loi sur la résilience opérationnelle numérique (DORA). Bien que ce cadre offre des indications précieuses, il est important de noter que les exigences juridiques énoncées dans la DORA elle-même restent de premier plan.
+Lien : https://www.norea.nl/dora</t>
   </si>
 </sst>
 </file>
@@ -3502,7 +3503,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3599,12 +3600,12 @@
         <v>313</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>311</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>314</v>
+        <v>556</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -3612,7 +3613,7 @@
         <v>312</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -3624,8 +3625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3714,12 +3715,12 @@
         <v>313</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>311</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>314</v>
+        <v>556</v>
       </c>
     </row>
   </sheetData>
@@ -3768,10 +3769,10 @@
         <v>33</v>
       </c>
       <c r="G1" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="H1" s="26" t="s">
         <v>316</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -3787,10 +3788,10 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H2" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -3806,10 +3807,10 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="218.4" x14ac:dyDescent="0.3">
@@ -3832,10 +3833,10 @@
         <v>40</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
@@ -3858,10 +3859,10 @@
         <v>40</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="405.6" x14ac:dyDescent="0.3">
@@ -3884,10 +3885,10 @@
         <v>40</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
@@ -3910,10 +3911,10 @@
         <v>40</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
@@ -3936,10 +3937,10 @@
         <v>40</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -3955,10 +3956,10 @@
       <c r="E9" s="5"/>
       <c r="F9" s="8"/>
       <c r="G9" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
@@ -3981,10 +3982,10 @@
         <v>52</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
@@ -4007,10 +4008,10 @@
         <v>52</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
@@ -4033,10 +4034,10 @@
         <v>52</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H12" s="27" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
@@ -4059,10 +4060,10 @@
         <v>52</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H13" s="27" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
@@ -4085,10 +4086,10 @@
         <v>52</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
@@ -4111,10 +4112,10 @@
         <v>52</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4130,10 +4131,10 @@
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
       <c r="G16" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H16" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -4156,10 +4157,10 @@
         <v>66</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -4182,10 +4183,10 @@
         <v>66</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H18" s="27" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -4208,10 +4209,10 @@
         <v>66</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4227,10 +4228,10 @@
       <c r="E20" s="7"/>
       <c r="F20" s="8"/>
       <c r="G20" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H20" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="124.8" x14ac:dyDescent="0.3">
@@ -4253,10 +4254,10 @@
         <v>74</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H21" s="27" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="124.8" x14ac:dyDescent="0.3">
@@ -4279,10 +4280,10 @@
         <v>74</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -4305,10 +4306,10 @@
         <v>74</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="202.8" x14ac:dyDescent="0.3">
@@ -4331,10 +4332,10 @@
         <v>74</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H24" s="27" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4350,10 +4351,10 @@
       <c r="E25" s="7"/>
       <c r="F25" s="10"/>
       <c r="G25" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4369,10 +4370,10 @@
       <c r="E26" s="7"/>
       <c r="F26" s="10"/>
       <c r="G26" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -4395,10 +4396,10 @@
         <v>86</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="218.4" x14ac:dyDescent="0.3">
@@ -4421,10 +4422,10 @@
         <v>86</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H28" s="27" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
@@ -4447,10 +4448,10 @@
         <v>86</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H29" s="27" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4466,10 +4467,10 @@
       <c r="E30" s="5"/>
       <c r="F30" s="10"/>
       <c r="G30" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H30" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -4492,10 +4493,10 @@
         <v>94</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H31" s="27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -4518,10 +4519,10 @@
         <v>94</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H32" s="27" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -4544,10 +4545,10 @@
         <v>94</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H33" s="27" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -4570,10 +4571,10 @@
         <v>94</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H34" s="27" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4589,10 +4590,10 @@
       <c r="E35" s="5"/>
       <c r="F35" s="8"/>
       <c r="G35" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H35" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -4615,10 +4616,10 @@
         <v>104</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H36" s="27" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -4641,10 +4642,10 @@
         <v>104</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H37" s="27" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -4667,10 +4668,10 @@
         <v>104</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H38" s="27" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -4693,10 +4694,10 @@
         <v>104</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H39" s="27" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4712,10 +4713,10 @@
       <c r="E40" s="5"/>
       <c r="F40" s="8"/>
       <c r="G40" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H40" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4731,10 +4732,10 @@
       <c r="E41" s="5"/>
       <c r="F41" s="8"/>
       <c r="G41" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H41" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
@@ -4757,10 +4758,10 @@
         <v>116</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H42" s="27" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="374.4" x14ac:dyDescent="0.3">
@@ -4783,10 +4784,10 @@
         <v>116</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H43" s="27" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4802,10 +4803,10 @@
       <c r="E44" s="7"/>
       <c r="F44" s="8"/>
       <c r="G44" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H44" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="374.4" x14ac:dyDescent="0.3">
@@ -4828,10 +4829,10 @@
         <v>122</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H45" s="27" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="374.4" x14ac:dyDescent="0.3">
@@ -4854,10 +4855,10 @@
         <v>122</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H46" s="27" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="374.4" x14ac:dyDescent="0.3">
@@ -4880,10 +4881,10 @@
         <v>122</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H47" s="27" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="374.4" x14ac:dyDescent="0.3">
@@ -4906,10 +4907,10 @@
         <v>122</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H48" s="27" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="374.4" x14ac:dyDescent="0.3">
@@ -4932,10 +4933,10 @@
         <v>122</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H49" s="27" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="374.4" x14ac:dyDescent="0.3">
@@ -4958,10 +4959,10 @@
         <v>122</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4977,10 +4978,10 @@
       <c r="E51" s="7"/>
       <c r="F51" s="8"/>
       <c r="G51" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H51" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -4996,10 +4997,10 @@
       <c r="E52" s="7"/>
       <c r="F52" s="8"/>
       <c r="G52" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="280.8" x14ac:dyDescent="0.3">
@@ -5022,10 +5023,10 @@
         <v>137</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H53" s="27" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="280.8" x14ac:dyDescent="0.3">
@@ -5048,10 +5049,10 @@
         <v>137</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H54" s="27" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5067,10 +5068,10 @@
       <c r="E55" s="7"/>
       <c r="F55" s="8"/>
       <c r="G55" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H55" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="312" x14ac:dyDescent="0.3">
@@ -5093,10 +5094,10 @@
         <v>142</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H56" s="27" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="312" x14ac:dyDescent="0.3">
@@ -5119,10 +5120,10 @@
         <v>142</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H57" s="27" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="312" x14ac:dyDescent="0.3">
@@ -5145,10 +5146,10 @@
         <v>142</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H58" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5164,10 +5165,10 @@
       <c r="E59" s="7"/>
       <c r="F59" s="8"/>
       <c r="G59" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H59" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -5183,10 +5184,10 @@
       <c r="E60" s="7"/>
       <c r="F60" s="8"/>
       <c r="G60" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H60" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -5209,10 +5210,10 @@
         <v>152</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H61" s="27" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
@@ -5235,10 +5236,10 @@
         <v>152</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H62" s="27" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -5261,10 +5262,10 @@
         <v>152</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H63" s="27" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -5287,10 +5288,10 @@
         <v>152</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H64" s="27" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5306,10 +5307,10 @@
       <c r="E65" s="5"/>
       <c r="F65" s="8"/>
       <c r="G65" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H65" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="216" x14ac:dyDescent="0.3">
@@ -5332,10 +5333,10 @@
         <v>162</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H66" s="27" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -5358,10 +5359,10 @@
         <v>162</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H67" s="27" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5377,10 +5378,10 @@
       <c r="E68" s="7"/>
       <c r="F68" s="8"/>
       <c r="G68" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H68" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -5396,10 +5397,10 @@
       <c r="E69" s="7"/>
       <c r="F69" s="8"/>
       <c r="G69" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H69" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -5422,10 +5423,10 @@
         <v>170</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H70" s="27" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
@@ -5448,10 +5449,10 @@
         <v>170</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H71" s="27" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -5467,10 +5468,10 @@
       <c r="E72" s="7"/>
       <c r="F72" s="8"/>
       <c r="G72" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H72" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -5493,10 +5494,10 @@
         <v>176</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H73" s="27" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -5519,10 +5520,10 @@
         <v>176</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H74" s="27" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -5545,10 +5546,10 @@
         <v>176</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H75" s="27" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -5571,10 +5572,10 @@
         <v>176</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H76" s="27" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -5597,10 +5598,10 @@
         <v>176</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H77" s="27" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -5616,10 +5617,10 @@
       <c r="E78" s="7"/>
       <c r="F78" s="8"/>
       <c r="G78" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H78" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
@@ -5642,10 +5643,10 @@
         <v>188</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H79" s="27" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
@@ -5668,10 +5669,10 @@
         <v>188</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H80" s="27" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="216" x14ac:dyDescent="0.3">
@@ -5694,10 +5695,10 @@
         <v>188</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H81" s="27" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5713,10 +5714,10 @@
       <c r="E82" s="11"/>
       <c r="F82" s="8"/>
       <c r="G82" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H82" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="202.8" x14ac:dyDescent="0.3">
@@ -5739,10 +5740,10 @@
         <v>194</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H83" s="27" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="202.8" x14ac:dyDescent="0.3">
@@ -5765,10 +5766,10 @@
         <v>194</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H84" s="27" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="202.8" x14ac:dyDescent="0.3">
@@ -5791,10 +5792,10 @@
         <v>194</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H85" s="27" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="202.8" x14ac:dyDescent="0.3">
@@ -5817,10 +5818,10 @@
         <v>194</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H86" s="27" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="202.8" x14ac:dyDescent="0.3">
@@ -5843,10 +5844,10 @@
         <v>194</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H87" s="27" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="202.8" x14ac:dyDescent="0.3">
@@ -5869,10 +5870,10 @@
         <v>194</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H88" s="27" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5888,10 +5889,10 @@
       <c r="E89" s="7"/>
       <c r="F89" s="8"/>
       <c r="G89" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H89" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="218.4" x14ac:dyDescent="0.3">
@@ -5914,10 +5915,10 @@
         <v>208</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H90" s="27" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="218.4" x14ac:dyDescent="0.3">
@@ -5940,10 +5941,10 @@
         <v>208</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H91" s="27" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="218.4" x14ac:dyDescent="0.3">
@@ -5966,10 +5967,10 @@
         <v>208</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H92" s="27" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -5985,10 +5986,10 @@
       <c r="E93" s="12"/>
       <c r="F93" s="8"/>
       <c r="G93" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H93" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -6004,10 +6005,10 @@
       <c r="E94" s="12"/>
       <c r="F94" s="8"/>
       <c r="G94" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H94" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
@@ -6030,10 +6031,10 @@
         <v>218</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H95" s="27" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
@@ -6056,10 +6057,10 @@
         <v>218</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H96" s="27" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="312" x14ac:dyDescent="0.3">
@@ -6082,10 +6083,10 @@
         <v>223</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H97" s="27" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -6101,10 +6102,10 @@
       <c r="E98" s="7"/>
       <c r="F98" s="8"/>
       <c r="G98" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H98" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="312" x14ac:dyDescent="0.3">
@@ -6127,10 +6128,10 @@
         <v>223</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H99" s="27" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="312" x14ac:dyDescent="0.3">
@@ -6153,10 +6154,10 @@
         <v>223</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H100" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -6172,10 +6173,10 @@
       <c r="E101" s="7"/>
       <c r="F101" s="8"/>
       <c r="G101" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H101" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -6191,10 +6192,10 @@
       <c r="E102" s="7"/>
       <c r="F102" s="8"/>
       <c r="G102" s="13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H102" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
@@ -6217,10 +6218,10 @@
         <v>234</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H103" s="27" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -6243,10 +6244,10 @@
         <v>234</v>
       </c>
       <c r="G104" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H104" s="27" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -6269,10 +6270,10 @@
         <v>234</v>
       </c>
       <c r="G105" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H105" s="27" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -6288,10 +6289,10 @@
       <c r="E106" s="7"/>
       <c r="F106" s="8"/>
       <c r="G106" s="13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H106" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="156" x14ac:dyDescent="0.3">
@@ -6314,10 +6315,10 @@
         <v>242</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H107" s="27" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="156" x14ac:dyDescent="0.3">
@@ -6340,10 +6341,10 @@
         <v>242</v>
       </c>
       <c r="G108" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H108" s="27" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="156" x14ac:dyDescent="0.3">
@@ -6366,10 +6367,10 @@
         <v>242</v>
       </c>
       <c r="G109" s="14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H109" s="27" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -6385,10 +6386,10 @@
       <c r="E110" s="5"/>
       <c r="F110" s="8"/>
       <c r="G110" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H110" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -6411,10 +6412,10 @@
         <v>250</v>
       </c>
       <c r="G111" s="14" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H111" s="27" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
@@ -6437,10 +6438,10 @@
         <v>250</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H112" s="27" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -6463,10 +6464,10 @@
         <v>250</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H113" s="27" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
@@ -6489,10 +6490,10 @@
         <v>250</v>
       </c>
       <c r="G114" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H114" s="27" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -6515,10 +6516,10 @@
         <v>250</v>
       </c>
       <c r="G115" s="14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H115" s="27" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -6534,10 +6535,10 @@
       <c r="E116" s="7"/>
       <c r="F116" s="8"/>
       <c r="G116" s="13" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H116" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="156" x14ac:dyDescent="0.3">
@@ -6560,10 +6561,10 @@
         <v>262</v>
       </c>
       <c r="G117" s="14" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H117" s="27" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
@@ -6586,10 +6587,10 @@
         <v>262</v>
       </c>
       <c r="G118" s="14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H118" s="27" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -6605,10 +6606,10 @@
       <c r="E119" s="5"/>
       <c r="F119" s="8"/>
       <c r="G119" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H119" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -6631,10 +6632,10 @@
         <v>268</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H120" s="27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -6657,10 +6658,10 @@
         <v>268</v>
       </c>
       <c r="G121" s="14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H121" s="27" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -6683,10 +6684,10 @@
         <v>268</v>
       </c>
       <c r="G122" s="14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H122" s="27" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
@@ -6709,10 +6710,10 @@
         <v>268</v>
       </c>
       <c r="G123" s="14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H123" s="27" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -6728,10 +6729,10 @@
       <c r="E124" s="7"/>
       <c r="F124" s="8"/>
       <c r="G124" s="14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H124" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
@@ -6754,10 +6755,10 @@
         <v>268</v>
       </c>
       <c r="G125" s="14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H125" s="27" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -6773,10 +6774,10 @@
       <c r="E126" s="7"/>
       <c r="F126" s="8"/>
       <c r="G126" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H126" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
@@ -6799,10 +6800,10 @@
         <v>280</v>
       </c>
       <c r="G127" s="14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H127" s="27" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -6825,10 +6826,10 @@
         <v>280</v>
       </c>
       <c r="G128" s="14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H128" s="27" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -6844,10 +6845,10 @@
       <c r="E129" s="5"/>
       <c r="F129" s="8"/>
       <c r="G129" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H129" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -6870,10 +6871,10 @@
         <v>286</v>
       </c>
       <c r="G130" s="15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H130" s="27" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="202.8" x14ac:dyDescent="0.3">
@@ -6896,10 +6897,10 @@
         <v>286</v>
       </c>
       <c r="G131" s="14" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H131" s="27" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
@@ -6922,10 +6923,10 @@
         <v>286</v>
       </c>
       <c r="G132" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H132" s="27" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -6969,7 +6970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -6998,13 +6999,13 @@
         <v>33</v>
       </c>
       <c r="E1" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" s="39" t="s">
         <v>316</v>
       </c>
-      <c r="F1" s="39" t="s">
-        <v>317</v>
-      </c>
       <c r="G1" s="39" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -7021,10 +7022,10 @@
         <v>294</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>294</v>
@@ -7047,10 +7048,10 @@
         <v>295</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
@@ -7067,13 +7068,13 @@
         <v>300</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G4" s="41" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
@@ -7090,13 +7091,13 @@
         <v>303</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
@@ -7113,13 +7114,13 @@
         <v>306</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
@@ -7136,13 +7137,13 @@
         <v>309</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G7" s="41" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>